<commit_message>
size corrected respirometry data
</commit_message>
<xml_diff>
--- a/respirometry/output/respirometry_summary.xlsx
+++ b/respirometry/output/respirometry_summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Respirometry\Desktop\FISH441\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Respirometry\Desktop\fish541_lab\respirometry\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E0E673A-2CC7-407A-BB66-E1C3D6A9A8D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9286B9AE-6A47-4352-A816-26C89B0D1AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{449C3B01-0FCE-4591-A807-44779BAD5345}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="50">
   <si>
     <t>mussel_ID</t>
   </si>
@@ -179,6 +179,12 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>SL_cm</t>
+  </si>
+  <si>
+    <t>umol_L_hr_cm</t>
   </si>
 </sst>
 </file>
@@ -222,7 +228,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -232,6 +238,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -547,11 +557,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F39EEFE-DAE0-4470-BF3D-6803FF603516}">
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H43" sqref="H43"/>
+      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -562,9 +572,11 @@
     <col min="4" max="4" width="8.83984375" style="1"/>
     <col min="5" max="5" width="13.89453125" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.3671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83984375" style="1"/>
+    <col min="8" max="8" width="12.62890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -583,8 +595,14 @@
       <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -603,8 +621,15 @@
       <c r="F2" s="1">
         <v>9.4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G2" s="1">
+        <v>6.4580000000000002</v>
+      </c>
+      <c r="H2">
+        <f>F2/G2</f>
+        <v>1.4555589965933726</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -623,8 +648,15 @@
       <c r="F3" s="1">
         <v>16.899999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G3" s="1">
+        <v>6.4580000000000002</v>
+      </c>
+      <c r="H3" s="4">
+        <f t="shared" ref="H3:H51" si="0">F3/G3</f>
+        <v>2.6169092598327652</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -643,8 +675,15 @@
       <c r="F4" s="1">
         <v>10.6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G4" s="5">
+        <v>6.7690000000000001</v>
+      </c>
+      <c r="H4" s="4">
+        <f t="shared" si="0"/>
+        <v>1.5659624759934998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -663,8 +702,15 @@
       <c r="F5" s="1">
         <v>56.2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G5" s="5">
+        <v>6.7690000000000001</v>
+      </c>
+      <c r="H5" s="4">
+        <f t="shared" si="0"/>
+        <v>8.302555768946668</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
@@ -683,8 +729,15 @@
       <c r="F6" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G6" s="5">
+        <v>5.1040000000000001</v>
+      </c>
+      <c r="H6" s="4">
+        <f t="shared" si="0"/>
+        <v>2.1551724137931032</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -703,8 +756,15 @@
       <c r="F7" s="1">
         <v>41.1</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G7" s="5">
+        <v>5.1040000000000001</v>
+      </c>
+      <c r="H7" s="4">
+        <f t="shared" si="0"/>
+        <v>8.0525078369905962</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -723,8 +783,9 @@
       <c r="F8" s="1">
         <v>9.6</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
@@ -743,8 +804,15 @@
       <c r="F9" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G9" s="5">
+        <v>5.3140000000000001</v>
+      </c>
+      <c r="H9" s="4">
+        <f t="shared" si="0"/>
+        <v>1.6936394429808055</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -763,8 +831,15 @@
       <c r="F10" s="1">
         <v>30.4</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G10" s="5">
+        <v>5.3140000000000001</v>
+      </c>
+      <c r="H10" s="4">
+        <f t="shared" si="0"/>
+        <v>5.7207376740684976</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -783,8 +858,15 @@
       <c r="F11" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G11" s="5">
+        <v>6.5620000000000003</v>
+      </c>
+      <c r="H11" s="4">
+        <f t="shared" si="0"/>
+        <v>0.76196281621456874</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
         <v>20</v>
       </c>
@@ -803,8 +885,15 @@
       <c r="F12" s="1">
         <v>25.7</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G12" s="5">
+        <v>6.5620000000000003</v>
+      </c>
+      <c r="H12" s="4">
+        <f t="shared" si="0"/>
+        <v>3.9164888753428828</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
         <v>21</v>
       </c>
@@ -823,8 +912,9 @@
       <c r="F13" s="1">
         <v>8.6999999999999993</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
@@ -843,8 +933,15 @@
       <c r="F14" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G14" s="5">
+        <v>6.5640000000000001</v>
+      </c>
+      <c r="H14" s="4">
+        <f t="shared" si="0"/>
+        <v>2.7422303473491771</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
@@ -863,8 +960,15 @@
       <c r="F15" s="1">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G15" s="5">
+        <v>6.3540000000000001</v>
+      </c>
+      <c r="H15" s="4">
+        <f t="shared" si="0"/>
+        <v>2.8328611898016995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
         <v>23</v>
       </c>
@@ -883,8 +987,15 @@
       <c r="F16" s="1">
         <v>17.100000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G16" s="5">
+        <v>6.3540000000000001</v>
+      </c>
+      <c r="H16" s="4">
+        <f t="shared" si="0"/>
+        <v>2.6912181303116149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
@@ -903,8 +1014,15 @@
       <c r="F17" s="1">
         <v>10.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G17" s="5">
+        <v>5.9359999999999999</v>
+      </c>
+      <c r="H17" s="4">
+        <f t="shared" si="0"/>
+        <v>1.7688679245283019</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
         <v>6</v>
       </c>
@@ -923,8 +1041,15 @@
       <c r="F18" s="1">
         <v>15.1</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G18" s="5">
+        <v>6.3540000000000001</v>
+      </c>
+      <c r="H18" s="4">
+        <f t="shared" si="0"/>
+        <v>2.3764557758892035</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
@@ -943,8 +1068,15 @@
       <c r="F19" s="1">
         <v>17.100000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G19" s="5">
+        <v>6.3540000000000001</v>
+      </c>
+      <c r="H19" s="4">
+        <f t="shared" si="0"/>
+        <v>2.6912181303116149</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
@@ -963,8 +1095,15 @@
       <c r="F20" s="1">
         <v>35.1</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G20" s="5">
+        <v>7.5010000000000003</v>
+      </c>
+      <c r="H20" s="4">
+        <f t="shared" si="0"/>
+        <v>4.6793760831889077</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
@@ -983,8 +1122,15 @@
       <c r="F21" s="1">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G21" s="5">
+        <v>7.5010000000000003</v>
+      </c>
+      <c r="H21" s="4">
+        <f t="shared" si="0"/>
+        <v>3.7328356219170775</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
@@ -1003,8 +1149,9 @@
       <c r="F22" s="1">
         <v>24.4</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="H22" s="4"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="1" t="s">
         <v>9</v>
       </c>
@@ -1023,8 +1170,15 @@
       <c r="F23" s="1">
         <v>21.3</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G23" s="5">
+        <v>6.5590000000000002</v>
+      </c>
+      <c r="H23" s="4">
+        <f t="shared" si="0"/>
+        <v>3.2474462570513798</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1" t="s">
         <v>9</v>
       </c>
@@ -1043,8 +1197,15 @@
       <c r="F24" s="1">
         <v>25.6</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G24" s="5">
+        <v>6.5590000000000002</v>
+      </c>
+      <c r="H24" s="4">
+        <f t="shared" si="0"/>
+        <v>3.9030339990852267</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1" t="s">
         <v>10</v>
       </c>
@@ -1063,8 +1224,15 @@
       <c r="F25" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G25" s="5">
+        <v>5.7320000000000002</v>
+      </c>
+      <c r="H25" s="4">
+        <f t="shared" si="0"/>
+        <v>0.87229588276343328</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1" t="s">
         <v>10</v>
       </c>
@@ -1083,8 +1251,15 @@
       <c r="F26" s="1">
         <v>14.2</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G26" s="5">
+        <v>5.7320000000000002</v>
+      </c>
+      <c r="H26" s="4">
+        <f t="shared" si="0"/>
+        <v>2.4773203070481506</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="1" t="s">
         <v>11</v>
       </c>
@@ -1103,8 +1278,15 @@
       <c r="F27" s="1">
         <v>31.9</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G27" s="5">
+        <v>6.0419999999999998</v>
+      </c>
+      <c r="H27" s="4">
+        <f t="shared" si="0"/>
+        <v>5.2797087057265806</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="1" t="s">
         <v>11</v>
       </c>
@@ -1123,8 +1305,15 @@
       <c r="F28" s="1">
         <v>6.6</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G28" s="5">
+        <v>6.0419999999999998</v>
+      </c>
+      <c r="H28" s="4">
+        <f t="shared" si="0"/>
+        <v>1.0923535253227408</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="1" t="s">
         <v>12</v>
       </c>
@@ -1143,8 +1332,15 @@
       <c r="F29" s="1">
         <v>2.2999999999999998</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G29" s="5">
+        <v>6.2509999999999994</v>
+      </c>
+      <c r="H29" s="4">
+        <f t="shared" si="0"/>
+        <v>0.36794112941929291</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1" t="s">
         <v>12</v>
       </c>
@@ -1163,8 +1359,15 @@
       <c r="F30" s="1">
         <v>12.7</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G30" s="5">
+        <v>6.2509999999999994</v>
+      </c>
+      <c r="H30" s="4">
+        <f t="shared" si="0"/>
+        <v>2.0316749320108785</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1" t="s">
         <v>13</v>
       </c>
@@ -1183,8 +1386,15 @@
       <c r="F31" s="1">
         <v>9.8000000000000007</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G31" s="5">
+        <v>6.4560000000000004</v>
+      </c>
+      <c r="H31" s="4">
+        <f t="shared" si="0"/>
+        <v>1.5179677819083024</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1" t="s">
         <v>14</v>
       </c>
@@ -1203,8 +1413,15 @@
       <c r="F32" s="1">
         <v>3.8</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G32" s="5">
+        <v>6.2469999999999999</v>
+      </c>
+      <c r="H32" s="4">
+        <f t="shared" si="0"/>
+        <v>0.60829198015047226</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="1" t="s">
         <v>14</v>
       </c>
@@ -1223,8 +1440,15 @@
       <c r="F33" s="1">
         <v>15.7</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G33" s="5">
+        <v>6.2469999999999999</v>
+      </c>
+      <c r="H33" s="4">
+        <f t="shared" si="0"/>
+        <v>2.5132063390427404</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="1" t="s">
         <v>16</v>
       </c>
@@ -1243,8 +1467,15 @@
       <c r="F34" s="1">
         <v>19.100000000000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G34" s="5">
+        <v>5.9380000000000006</v>
+      </c>
+      <c r="H34" s="4">
+        <f t="shared" si="0"/>
+        <v>3.2165712361064331</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="1" t="s">
         <v>16</v>
       </c>
@@ -1263,8 +1494,15 @@
       <c r="F35" s="1">
         <v>15.2</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G35" s="5">
+        <v>5.9380000000000006</v>
+      </c>
+      <c r="H35" s="4">
+        <f t="shared" si="0"/>
+        <v>2.559784439205119</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="1" t="s">
         <v>35</v>
       </c>
@@ -1283,8 +1521,15 @@
       <c r="F36" s="1">
         <v>15.4</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G36" s="5">
+        <v>5.2119999999999997</v>
+      </c>
+      <c r="H36" s="4">
+        <f t="shared" si="0"/>
+        <v>2.9547198772064469</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="1" t="s">
         <v>36</v>
       </c>
@@ -1303,8 +1548,15 @@
       <c r="F37" s="1">
         <v>16.3</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G37" s="5">
+        <v>5.9380000000000006</v>
+      </c>
+      <c r="H37" s="4">
+        <f t="shared" si="0"/>
+        <v>2.7450319973054897</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="1" t="s">
         <v>37</v>
       </c>
@@ -1323,8 +1575,15 @@
       <c r="F38" s="1">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G38" s="5">
+        <v>6.4590000000000005</v>
+      </c>
+      <c r="H38" s="4">
+        <f t="shared" si="0"/>
+        <v>0.83604273107292149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -1343,8 +1602,15 @@
       <c r="F39" s="1">
         <v>16.899999999999999</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G39" s="5">
+        <v>5.3119999999999994</v>
+      </c>
+      <c r="H39" s="4">
+        <f t="shared" si="0"/>
+        <v>3.1814759036144578</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="1" t="s">
         <v>39</v>
       </c>
@@ -1363,8 +1629,15 @@
       <c r="F40" s="1">
         <v>19.5</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G40" s="5">
+        <v>5.4169999999999998</v>
+      </c>
+      <c r="H40" s="4">
+        <f t="shared" si="0"/>
+        <v>3.5997784751707589</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="1" t="s">
         <v>24</v>
       </c>
@@ -1383,8 +1656,15 @@
       <c r="F41" s="1">
         <v>33.299999999999997</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G41" s="5">
+        <v>5.9380000000000006</v>
+      </c>
+      <c r="H41" s="4">
+        <f t="shared" si="0"/>
+        <v>5.6079488043112145</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1" t="s">
         <v>25</v>
       </c>
@@ -1403,8 +1683,15 @@
       <c r="F42" s="1">
         <v>18.899999999999999</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G42" s="5">
+        <v>6.6659999999999995</v>
+      </c>
+      <c r="H42" s="4">
+        <f t="shared" si="0"/>
+        <v>2.8352835283528353</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1" t="s">
         <v>26</v>
       </c>
@@ -1423,8 +1710,15 @@
       <c r="F43" s="1">
         <v>23.9</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G43" s="5">
+        <v>6.875</v>
+      </c>
+      <c r="H43" s="4">
+        <f t="shared" si="0"/>
+        <v>3.4763636363636361</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="1" t="s">
         <v>27</v>
       </c>
@@ -1443,8 +1737,15 @@
       <c r="F44" s="1">
         <v>33.299999999999997</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G44" s="5">
+        <v>6.5620000000000003</v>
+      </c>
+      <c r="H44" s="4">
+        <f t="shared" si="0"/>
+        <v>5.0746723559890272</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="1" t="s">
         <v>28</v>
       </c>
@@ -1463,8 +1764,15 @@
       <c r="F45" s="1">
         <v>32.9</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G45" s="5">
+        <v>6.1450000000000005</v>
+      </c>
+      <c r="H45" s="4">
+        <f t="shared" si="0"/>
+        <v>5.3539462978030912</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="1" t="s">
         <v>29</v>
       </c>
@@ -1483,8 +1791,15 @@
       <c r="F46" s="1">
         <v>12.8</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G46" s="5">
+        <v>6.3540000000000001</v>
+      </c>
+      <c r="H46" s="4">
+        <f t="shared" si="0"/>
+        <v>2.014479068303431</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="1" t="s">
         <v>30</v>
       </c>
@@ -1503,8 +1818,15 @@
       <c r="F47" s="1">
         <v>27.9</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G47" s="5">
+        <v>4.7919999999999998</v>
+      </c>
+      <c r="H47" s="4">
+        <f t="shared" si="0"/>
+        <v>5.82220367278798</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="1" t="s">
         <v>31</v>
       </c>
@@ -1523,8 +1845,15 @@
       <c r="F48" s="1">
         <v>16.100000000000001</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G48" s="5">
+        <v>5.5229999999999997</v>
+      </c>
+      <c r="H48" s="4">
+        <f t="shared" si="0"/>
+        <v>2.9150823827629915</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="1" t="s">
         <v>32</v>
       </c>
@@ -1543,8 +1872,15 @@
       <c r="F49" s="1">
         <v>41</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G49" s="5">
+        <v>6.1470000000000002</v>
+      </c>
+      <c r="H49" s="4">
+        <f t="shared" si="0"/>
+        <v>6.6699202863185292</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="1" t="s">
         <v>33</v>
       </c>
@@ -1563,8 +1899,15 @@
       <c r="F50" s="1">
         <v>40.200000000000003</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="G50" s="5">
+        <v>5.5200000000000005</v>
+      </c>
+      <c r="H50" s="4">
+        <f t="shared" si="0"/>
+        <v>7.2826086956521738</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="1" t="s">
         <v>34</v>
       </c>
@@ -1582,6 +1925,13 @@
       </c>
       <c r="F51" s="1">
         <v>23.1</v>
+      </c>
+      <c r="G51" s="5">
+        <v>6.25</v>
+      </c>
+      <c r="H51" s="4">
+        <f t="shared" si="0"/>
+        <v>3.6960000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>